<commit_message>
Flash_Fill, Text_to_columns, Find & Select
</commit_message>
<xml_diff>
--- a/Personal_Monthly_Expenditure_Lab4.xlsx
+++ b/Personal_Monthly_Expenditure_Lab4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvipi\Desktop\VIP_GitHub\MS-Excel_Learning_Journey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCB26EF-D067-4417-B827-F6583476366D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0CB0F1-8DEB-4096-AE58-E7FB2AAF7294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,7 +116,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -160,12 +160,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,195 +187,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -429,7 +240,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -456,7 +267,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -483,7 +294,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -510,7 +321,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -537,7 +348,195 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -618,13 +617,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AB075690-6493-4B96-8D1B-B29AB2D9E9A9}" name="Table6" displayName="Table6" ref="A1:H14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:H14" xr:uid="{1C96BD00-98D9-4572-8F4A-F406BBA95AE3}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0738465F-87B9-46AD-8314-585AF20E321C}" name="Month" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{639B5A90-C646-4312-A12B-90EBA415C5F3}" name="Housing" dataDxfId="6" totalsRowDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{AC863E34-6694-4292-A7E8-5D94B1D4B90E}" name="Bills &amp; Utilities" dataDxfId="5" totalsRowDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{7F96B093-000D-47C8-9B3D-9C6DC794A7DD}" name="Food &amp; Dining" dataDxfId="4" totalsRowDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{0D73BCA8-FF88-432A-8438-8D3C42615074}" name="Personal" dataDxfId="3" totalsRowDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{62ECB4B2-7FAC-4168-96E6-6A3296B9F2CB}" name="Auto &amp; Transport" dataDxfId="2" totalsRowDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{5C8E2143-EA5D-49A7-8A33-6E4F45D73494}" name="Health &amp; Fitness" dataDxfId="1" totalsRowDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{0738465F-87B9-46AD-8314-585AF20E321C}" name="Month" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{639B5A90-C646-4312-A12B-90EBA415C5F3}" name="Housing" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{AC863E34-6694-4292-A7E8-5D94B1D4B90E}" name="Bills &amp; Utilities" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{7F96B093-000D-47C8-9B3D-9C6DC794A7DD}" name="Food &amp; Dining" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{0D73BCA8-FF88-432A-8438-8D3C42615074}" name="Personal" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{62ECB4B2-7FAC-4168-96E6-6A3296B9F2CB}" name="Auto &amp; Transport" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{5C8E2143-EA5D-49A7-8A33-6E4F45D73494}" name="Health &amp; Fitness" dataDxfId="2" totalsRowDxfId="1"/>
     <tableColumn id="8" xr3:uid="{1BE4B897-B8F6-4FE8-9775-458649F106E7}" name="Monthly Total" dataDxfId="0">
       <calculatedColumnFormula>SUM(B2:G2)</calculatedColumnFormula>
     </tableColumn>
@@ -932,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -970,7 +969,7 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -996,7 +995,7 @@
       <c r="G2" s="3">
         <v>60</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <f t="shared" ref="H2:H14" si="0">SUM(B2:G2)</f>
         <v>1670</v>
       </c>
@@ -1023,7 +1022,7 @@
       <c r="G3" s="3">
         <v>70</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <f t="shared" si="0"/>
         <v>1625</v>
       </c>
@@ -1050,7 +1049,7 @@
       <c r="G4" s="3">
         <v>60</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <f t="shared" si="0"/>
         <v>1670</v>
       </c>
@@ -1077,7 +1076,7 @@
       <c r="G5" s="3">
         <v>60</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
         <v>1640</v>
       </c>
@@ -1104,7 +1103,7 @@
       <c r="G6" s="3">
         <v>80</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <f t="shared" si="0"/>
         <v>1650</v>
       </c>
@@ -1131,7 +1130,7 @@
       <c r="G7" s="3">
         <v>60</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <f t="shared" si="0"/>
         <v>1620</v>
       </c>
@@ -1158,7 +1157,7 @@
       <c r="G8" s="3">
         <v>60</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <f t="shared" si="0"/>
         <v>1650</v>
       </c>
@@ -1185,7 +1184,7 @@
       <c r="G9" s="3">
         <v>80</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <f t="shared" si="0"/>
         <v>1650</v>
       </c>
@@ -1212,7 +1211,7 @@
       <c r="G10" s="3">
         <v>60</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <f t="shared" si="0"/>
         <v>1640</v>
       </c>
@@ -1239,7 +1238,7 @@
       <c r="G11" s="3">
         <v>60</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <f t="shared" si="0"/>
         <v>1650</v>
       </c>
@@ -1266,7 +1265,7 @@
       <c r="G12" s="3">
         <v>50</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <f t="shared" si="0"/>
         <v>1660</v>
       </c>
@@ -1293,7 +1292,7 @@
       <c r="G13" s="3">
         <v>60</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <f t="shared" si="0"/>
         <v>1695</v>
       </c>
@@ -1302,31 +1301,31 @@
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <f>SUM(B2:B13)</f>
         <v>9600</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <f t="shared" ref="C14:G14" si="1">SUM(C2:C13)</f>
         <v>2060</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <f t="shared" si="1"/>
         <v>4820</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <f t="shared" si="1"/>
         <v>1280</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <f t="shared" si="1"/>
         <v>1300</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <f t="shared" si="1"/>
         <v>760</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <f t="shared" si="0"/>
         <v>19820</v>
       </c>
@@ -1519,7 +1518,7 @@
         <v>3</v>
       </c>
       <c r="D33" s="3">
-        <f>$A$31+$A32</f>
+        <f t="shared" ref="D33:D40" si="7">$A$31+$A32</f>
         <v>3</v>
       </c>
     </row>
@@ -1528,15 +1527,15 @@
         <v>4</v>
       </c>
       <c r="B34" s="3">
-        <f t="shared" ref="B34:B40" si="7">A32+A33</f>
+        <f t="shared" ref="B34:B40" si="8">A32+A33</f>
         <v>5</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" ref="C34:C40" si="8">$A$31+$A$32</f>
+        <f t="shared" ref="C34:C40" si="9">$A$31+$A$32</f>
         <v>3</v>
       </c>
       <c r="D34" s="3">
-        <f>$A$31+$A33</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
@@ -1545,15 +1544,15 @@
         <v>5</v>
       </c>
       <c r="B35" s="3">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="D35" s="3">
         <f t="shared" si="7"/>
-        <v>7</v>
-      </c>
-      <c r="C35" s="3">
-        <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="D35" s="3">
-        <f>$A$31+$A34</f>
         <v>5</v>
       </c>
     </row>
@@ -1562,15 +1561,15 @@
         <v>6</v>
       </c>
       <c r="B36" s="3">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="D36" s="3">
         <f t="shared" si="7"/>
-        <v>9</v>
-      </c>
-      <c r="C36" s="3">
-        <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="D36" s="3">
-        <f>$A$31+$A35</f>
         <v>6</v>
       </c>
     </row>
@@ -1579,15 +1578,15 @@
         <v>7</v>
       </c>
       <c r="B37" s="3">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="D37" s="3">
         <f t="shared" si="7"/>
-        <v>11</v>
-      </c>
-      <c r="C37" s="3">
-        <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="D37" s="3">
-        <f>$A$31+$A36</f>
         <v>7</v>
       </c>
     </row>
@@ -1596,15 +1595,15 @@
         <v>8</v>
       </c>
       <c r="B38" s="3">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="D38" s="3">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="C38" s="3">
-        <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="D38" s="3">
-        <f>$A$31+$A37</f>
         <v>8</v>
       </c>
     </row>
@@ -1613,15 +1612,15 @@
         <v>9</v>
       </c>
       <c r="B39" s="3">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="D39" s="3">
         <f t="shared" si="7"/>
-        <v>15</v>
-      </c>
-      <c r="C39" s="3">
-        <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="D39" s="3">
-        <f>$A$31+$A38</f>
         <v>9</v>
       </c>
     </row>
@@ -1630,15 +1629,15 @@
         <v>10</v>
       </c>
       <c r="B40" s="3">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="D40" s="3">
         <f t="shared" si="7"/>
-        <v>17</v>
-      </c>
-      <c r="C40" s="3">
-        <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="D40" s="3">
-        <f>$A$31+$A39</f>
         <v>10</v>
       </c>
     </row>

</xml_diff>